<commit_message>
re-organized folder, updates notebooks, and added to image processing and interacting with web
</commit_message>
<xml_diff>
--- a/Module_Data_Analysis/Data/College-Majors/recent_Arts_edited.xlsx
+++ b/Module_Data_Analysis/Data/College-Majors/recent_Arts_edited.xlsx
@@ -1,144 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arts" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Arts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Major_code</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Major_category</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Sample_size</t>
-  </si>
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>Women</t>
-  </si>
-  <si>
-    <t>ShareWomen</t>
-  </si>
-  <si>
-    <t>Employed</t>
-  </si>
-  <si>
-    <t>Full_time</t>
-  </si>
-  <si>
-    <t>Part_time</t>
-  </si>
-  <si>
-    <t>Full_time_year_round</t>
-  </si>
-  <si>
-    <t>Unemployed</t>
-  </si>
-  <si>
-    <t>Unemployment_rate</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>P25th</t>
-  </si>
-  <si>
-    <t>P75th</t>
-  </si>
-  <si>
-    <t>College_jobs</t>
-  </si>
-  <si>
-    <t>Non_college_jobs</t>
-  </si>
-  <si>
-    <t>Low_wage_jobs</t>
-  </si>
-  <si>
-    <t>Test_column</t>
-  </si>
-  <si>
-    <t>Percent_Employed</t>
-  </si>
-  <si>
-    <t>z_score_college_jobs</t>
-  </si>
-  <si>
-    <t>MISCELLANEOUS FINE ARTS</t>
-  </si>
-  <si>
-    <t>COMMERCIAL ART AND GRAPHIC DESIGN</t>
-  </si>
-  <si>
-    <t>FILM VIDEO AND PHOTOGRAPHIC ARTS</t>
-  </si>
-  <si>
-    <t>MUSIC</t>
-  </si>
-  <si>
-    <t>FINE ARTS</t>
-  </si>
-  <si>
-    <t>VISUAL AND PERFORMING ARTS</t>
-  </si>
-  <si>
-    <t>STUDIO ARTS</t>
-  </si>
-  <si>
-    <t>DRAMA AND THEATER ARTS</t>
-  </si>
-  <si>
-    <t>Arts</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -153,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -469,656 +420,750 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Major_code</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Major</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Major_category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sample_size</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Men</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ShareWomen</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Full_time</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Part_time</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Full_time_year_round</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Unemployment_rate</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>P25th</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>P75th</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>College_jobs</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Non_college_jobs</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Low_wage_jobs</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Test_column</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Percent_Employed</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>z_score_college_jobs</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>33</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>6099</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MISCELLANEOUS FINE ARTS</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>3340</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>30</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>1970</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>1370</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>0.410179641</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="n">
         <v>2914</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="n">
         <v>2049</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="n">
         <v>1067</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>1200</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="n">
         <v>286</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="n">
         <v>0.089375</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="n">
         <v>50000</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="n">
         <v>25000</v>
       </c>
-      <c r="R2">
+      <c r="R2" t="n">
         <v>66000</v>
       </c>
-      <c r="S2">
+      <c r="S2" t="n">
         <v>693</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="n">
         <v>1714</v>
       </c>
-      <c r="U2">
+      <c r="U2" t="n">
         <v>755</v>
       </c>
-      <c r="W2">
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="n">
         <v>87.24550898203593</v>
       </c>
-      <c r="X2">
+      <c r="X2" t="n">
         <v>-0.9194237894803576</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>96</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>6004</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>COMMERCIAL ART AND GRAPHIC DESIGN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>103480</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>1186</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>8617</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>5156</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>0.3743556229999999</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="n">
         <v>83483</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="n">
         <v>67448</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="n">
         <v>24387</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="n">
         <v>52243</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="n">
         <v>8947</v>
       </c>
-      <c r="O3">
+      <c r="O3" t="n">
         <v>0.096797577</v>
       </c>
-      <c r="P3">
+      <c r="P3" t="n">
         <v>35000</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" t="n">
         <v>25000</v>
       </c>
-      <c r="R3">
+      <c r="R3" t="n">
         <v>45000</v>
       </c>
-      <c r="S3">
+      <c r="S3" t="n">
         <v>37389</v>
       </c>
-      <c r="T3">
+      <c r="T3" t="n">
         <v>38119</v>
       </c>
-      <c r="U3">
+      <c r="U3" t="n">
         <v>14839</v>
       </c>
-      <c r="W3">
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="n">
         <v>80.67549284885968</v>
       </c>
-      <c r="X3">
+      <c r="X3" t="n">
         <v>2.105121016496375</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>142</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>6005</v>
       </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>FILM VIDEO AND PHOTOGRAPHIC ARTS</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>38761</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>331</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>22339</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>49030</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>0.686992952</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="n">
         <v>31433</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="n">
         <v>22457</v>
       </c>
-      <c r="L4">
+      <c r="L4" t="n">
         <v>12818</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="n">
         <v>15740</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="n">
         <v>3718</v>
       </c>
-      <c r="O4">
+      <c r="O4" t="n">
         <v>0.10577224</v>
       </c>
-      <c r="P4">
+      <c r="P4" t="n">
         <v>32000</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" t="n">
         <v>22000</v>
       </c>
-      <c r="R4">
+      <c r="R4" t="n">
         <v>42000</v>
       </c>
-      <c r="S4">
+      <c r="S4" t="n">
         <v>7368</v>
       </c>
-      <c r="T4">
+      <c r="T4" t="n">
         <v>20721</v>
       </c>
-      <c r="U4">
+      <c r="U4" t="n">
         <v>5862</v>
       </c>
-      <c r="W4">
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="n">
         <v>81.09439900931349</v>
       </c>
-      <c r="X4">
+      <c r="X4" t="n">
         <v>-0.3692592870851458</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>147</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>6002</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MUSIC</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>60633</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>419</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>15670</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>12543</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>0.444582285</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="n">
         <v>47662</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="n">
         <v>29010</v>
       </c>
-      <c r="L5">
+      <c r="L5" t="n">
         <v>24943</v>
       </c>
-      <c r="M5">
+      <c r="M5" t="n">
         <v>21425</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="n">
         <v>3918</v>
       </c>
-      <c r="O5">
+      <c r="O5" t="n">
         <v>0.075959674</v>
       </c>
-      <c r="P5">
+      <c r="P5" t="n">
         <v>31000</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" t="n">
         <v>22300</v>
       </c>
-      <c r="R5">
+      <c r="R5" t="n">
         <v>42000</v>
       </c>
-      <c r="S5">
+      <c r="S5" t="n">
         <v>13752</v>
       </c>
-      <c r="T5">
+      <c r="T5" t="n">
         <v>28786</v>
       </c>
-      <c r="U5">
+      <c r="U5" t="n">
         <v>9286</v>
       </c>
-      <c r="W5">
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="n">
         <v>78.60735902891165</v>
       </c>
-      <c r="X5">
+      <c r="X5" t="n">
         <v>0.1569205156550837</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" t="n">
         <v>150</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>6000</v>
       </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>FINE ARTS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>74440</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>623</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>24786</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>49654</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>0.667033853</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="n">
         <v>59679</v>
       </c>
-      <c r="K6">
+      <c r="K6" t="n">
         <v>42764</v>
       </c>
-      <c r="L6">
+      <c r="L6" t="n">
         <v>23656</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="n">
         <v>31877</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="n">
         <v>5486</v>
       </c>
-      <c r="O6">
+      <c r="O6" t="n">
         <v>0.08418629599999999</v>
       </c>
-      <c r="P6">
+      <c r="P6" t="n">
         <v>30500</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" t="n">
         <v>21000</v>
       </c>
-      <c r="R6">
+      <c r="R6" t="n">
         <v>41000</v>
       </c>
-      <c r="S6">
+      <c r="S6" t="n">
         <v>20792</v>
       </c>
-      <c r="T6">
+      <c r="T6" t="n">
         <v>32725</v>
       </c>
-      <c r="U6">
+      <c r="U6" t="n">
         <v>11880</v>
       </c>
-      <c r="W6">
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="n">
         <v>80.17060720042987</v>
       </c>
-      <c r="X6">
+      <c r="X6" t="n">
         <v>0.737168919679397</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7">
+    <row r="7">
+      <c r="A7" t="n">
         <v>154</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>6003</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>VISUAL AND PERFORMING ARTS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>16250</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>132</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>2013</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>4639</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>0.697384245</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="n">
         <v>12870</v>
       </c>
-      <c r="K7">
+      <c r="K7" t="n">
         <v>8447</v>
       </c>
-      <c r="L7">
+      <c r="L7" t="n">
         <v>6253</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="n">
         <v>6322</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="n">
         <v>1465</v>
       </c>
-      <c r="O7">
+      <c r="O7" t="n">
         <v>0.102197419</v>
       </c>
-      <c r="P7">
+      <c r="P7" t="n">
         <v>30000</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" t="n">
         <v>22000</v>
       </c>
-      <c r="R7">
+      <c r="R7" t="n">
         <v>40000</v>
       </c>
-      <c r="S7">
+      <c r="S7" t="n">
         <v>3849</v>
       </c>
-      <c r="T7">
+      <c r="T7" t="n">
         <v>7635</v>
       </c>
-      <c r="U7">
+      <c r="U7" t="n">
         <v>2840</v>
       </c>
-      <c r="W7">
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="n">
         <v>79.2</v>
       </c>
-      <c r="X7">
+      <c r="X7" t="n">
         <v>-0.6593010674490036</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
-      <c r="A8">
+    <row r="8">
+      <c r="A8" t="n">
         <v>160</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>6007</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>STUDIO ARTS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>16977</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>182</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>4364</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>6146</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="n">
         <v>0.584776403</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="n">
         <v>13908</v>
       </c>
-      <c r="K8">
+      <c r="K8" t="n">
         <v>10451</v>
       </c>
-      <c r="L8">
+      <c r="L8" t="n">
         <v>5673</v>
       </c>
-      <c r="M8">
+      <c r="M8" t="n">
         <v>7413</v>
       </c>
-      <c r="N8">
+      <c r="N8" t="n">
         <v>1368</v>
       </c>
-      <c r="O8">
+      <c r="O8" t="n">
         <v>0.08955223900000001</v>
       </c>
-      <c r="P8">
+      <c r="P8" t="n">
         <v>29000</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" t="n">
         <v>19200</v>
       </c>
-      <c r="R8">
+      <c r="R8" t="n">
         <v>38300</v>
       </c>
-      <c r="S8">
+      <c r="S8" t="n">
         <v>3948</v>
       </c>
-      <c r="T8">
+      <c r="T8" t="n">
         <v>8707</v>
       </c>
-      <c r="U8">
+      <c r="U8" t="n">
         <v>3586</v>
       </c>
-      <c r="W8">
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="n">
         <v>81.9226011662838</v>
       </c>
-      <c r="X8">
+      <c r="X8" t="n">
         <v>-0.6511413242674117</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
-      <c r="A9">
+    <row r="9">
+      <c r="A9" t="n">
         <v>167</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>6001</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DRAMA AND THEATER ARTS</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>43249</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>357</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>7022</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>11931</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>0.629504564</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="n">
         <v>36165</v>
       </c>
-      <c r="K9">
+      <c r="K9" t="n">
         <v>25147</v>
       </c>
-      <c r="L9">
+      <c r="L9" t="n">
         <v>15994</v>
       </c>
-      <c r="M9">
+      <c r="M9" t="n">
         <v>16891</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="n">
         <v>3040</v>
       </c>
-      <c r="O9">
+      <c r="O9" t="n">
         <v>0.07754113</v>
       </c>
-      <c r="P9">
+      <c r="P9" t="n">
         <v>27000</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" t="n">
         <v>19200</v>
       </c>
-      <c r="R9">
+      <c r="R9" t="n">
         <v>35000</v>
       </c>
-      <c r="S9">
+      <c r="S9" t="n">
         <v>6994</v>
       </c>
-      <c r="T9">
+      <c r="T9" t="n">
         <v>25313</v>
       </c>
-      <c r="U9">
+      <c r="U9" t="n">
         <v>11068</v>
       </c>
-      <c r="W9">
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="n">
         <v>83.62043053018567</v>
       </c>
-      <c r="X9">
+      <c r="X9" t="n">
         <v>-0.4000849835489375</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>